<commit_message>
"comparing two excel files and creating a new file called with status and reason column"
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,40 +1,187 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+  <si>
+    <t>SO AR Details for Business Unit Optical OEM/ODM (PL)</t>
+  </si>
+  <si>
+    <t>Unnamed: 1</t>
+  </si>
+  <si>
+    <t>Unnamed: 2</t>
+  </si>
+  <si>
+    <t>Unnamed: 3</t>
+  </si>
+  <si>
+    <t>Unnamed: 4</t>
+  </si>
+  <si>
+    <t>Unnamed: 5</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>https://qmskpi-test.app.nokia.com/apps/qmmpro/reports/tl9prodmetrics.aspx?metric=SO&amp;type=detail&amp;sdate=2022-01&amp;edate=2024-01&amp;ver=45&amp;pu=L60800&amp;pt=pu</t>
+  </si>
+  <si>
+    <t>Data is PROPRIETARY and should not be shared with Customer unless verified</t>
+  </si>
+  <si>
+    <t>Report generated:Wednesday, January 17, 2024 11:31:12 PM Central Time</t>
+  </si>
+  <si>
+    <t>TECHNOLOGY NAME</t>
+  </si>
+  <si>
+    <t>NI - Optical Networks (BU)</t>
+  </si>
+  <si>
+    <t>NI - Optical Fiber Networks (BU)</t>
+  </si>
+  <si>
+    <t>AR NUMBER</t>
+  </si>
+  <si>
+    <t>2348179</t>
+  </si>
+  <si>
+    <t>2537472</t>
+  </si>
+  <si>
+    <t>2914075</t>
+  </si>
+  <si>
+    <t>2914014</t>
+  </si>
+  <si>
+    <t>2915777</t>
+  </si>
+  <si>
+    <t>2982457</t>
+  </si>
+  <si>
+    <t>3097451</t>
+  </si>
+  <si>
+    <t>3160819</t>
+  </si>
+  <si>
+    <t>999099</t>
+  </si>
+  <si>
+    <t>3510747</t>
+  </si>
+  <si>
+    <t>ACTUAL REPORTED DATE</t>
+  </si>
+  <si>
+    <t>04-27-2023  22:49:04</t>
+  </si>
+  <si>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>1830 SMS</t>
+  </si>
+  <si>
+    <t>WaveLite</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>1830 ONE</t>
+  </si>
+  <si>
+    <t>SO OUTAGE UNITS</t>
+  </si>
+  <si>
+    <t>SO1EA</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Not Matching</t>
+  </si>
+  <si>
+    <t>Matching</t>
+  </si>
+  <si>
+    <t>Unnamed: 1, Unnamed: 2, Unnamed: 3, Unnamed: 4, Unnamed: 5</t>
+  </si>
+  <si>
+    <t>Unnamed: 1, Unnamed: 3</t>
+  </si>
+  <si>
+    <t>SO AR Details for Business Unit Optical OEM/ODM (PL), Unnamed: 5</t>
+  </si>
+  <si>
+    <t>Unnamed: 2, Unnamed: 5</t>
+  </si>
+  <si>
+    <t>Unnamed: 2, Unnamed: 3, Unnamed: 5</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <scheme val="minor"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,85 +189,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -408,21 +513,370 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1"/>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44598.26166666667</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3">
+        <v>44738.93460648148</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>0.84807</v>
+      </c>
+      <c r="F7">
+        <v>0.84807</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44978.77878472222</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>0.84807</v>
+      </c>
+      <c r="F8">
+        <v>0.84807</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44978.77878472222</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <v>0.84807</v>
+      </c>
+      <c r="F9">
+        <v>0.84807</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <v>3.3923</v>
+      </c>
+      <c r="F10">
+        <v>99</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45014.79848379629</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>2.95384</v>
+      </c>
+      <c r="F11">
+        <v>2.95384</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45078.78480324074</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12">
+        <v>84.80744</v>
+      </c>
+      <c r="F12">
+        <v>84.80744</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13">
+        <v>2.724</v>
+      </c>
+      <c r="F13">
+        <v>25.724</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45111.95074074074</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>2.724</v>
+      </c>
+      <c r="F14">
+        <v>2.724</v>
+      </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45271.72056712963</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15">
+        <v>0.84807</v>
+      </c>
+      <c r="F15">
+        <v>0.84807</v>
+      </c>
+      <c r="G15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45271.72056712963</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16">
+        <v>0.84807</v>
+      </c>
+      <c r="F16">
+        <v>0.84807</v>
+      </c>
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>